<commit_message>
Add initial manual test cases Excel file
</commit_message>
<xml_diff>
--- a/test_cases/manual_test_cases.xlsx
+++ b/test_cases/manual_test_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leilabeigi/medical-device-qa-simulation/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7859A0C8-D23E-2242-8D3A-CD36DAF0CF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{858F1860-00C6-C642-994F-6644C8B94A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual Test Cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -28,81 +28,187 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Preconditions</t>
-  </si>
-  <si>
-    <t>Steps</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
+    <t>TC-001</t>
+  </si>
+  <si>
+    <t>Verify correct insulin dose is delivered based on user-configured units</t>
+  </si>
+  <si>
+    <t>TC-002</t>
+  </si>
+  <si>
+    <t>Verify mobile app displays last 5 doses</t>
+  </si>
+  <si>
+    <t>TC-003</t>
+  </si>
+  <si>
+    <t>Verify mobile app displays battery level</t>
+  </si>
+  <si>
+    <t>TC-004</t>
+  </si>
+  <si>
+    <t>Verify alert when battery level falls below 10%</t>
+  </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>Verify dosage history is stored for 30 days</t>
+  </si>
+  <si>
+    <t>TC-006</t>
+  </si>
+  <si>
+    <t>Verify all patient data is encrypted and stored locally</t>
+  </si>
+  <si>
+    <t>TC-007</t>
+  </si>
+  <si>
+    <t>Verify vibration and LED notification on critical alerts</t>
+  </si>
+  <si>
+    <t>TC-008</t>
+  </si>
+  <si>
+    <t>Verify login with valid credentials</t>
+  </si>
+  <si>
+    <t>TC-009</t>
+  </si>
+  <si>
+    <t>Verify login with invalid password</t>
+  </si>
+  <si>
+    <t>TC-010</t>
+  </si>
+  <si>
+    <t>Verify password reset process</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>Verify login with valid credentials</t>
-  </si>
-  <si>
-    <t>User has an account</t>
-  </si>
-  <si>
-    <t>1. Go to login page
-2. Enter valid credentials
-3. Click login</t>
-  </si>
-  <si>
-    <t>User is redirected to dashboard</t>
-  </si>
-  <si>
     <t>Not Executed</t>
   </si>
   <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>Verify login with invalid password</t>
-  </si>
-  <si>
-    <t>1. Go to login page
-2. Enter valid email
-3. Enter wrong password
-4. Click login</t>
-  </si>
-  <si>
-    <t>Error message is displayed</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>Verify password reset</t>
-  </si>
-  <si>
-    <t>1. Click on 'Forgot Password'
-2. Enter registered email
-3. Check inbox for reset link</t>
-  </si>
-  <si>
-    <t>Password reset email is received</t>
+    <t>User has configured insulin units</t>
+  </si>
+  <si>
+    <t>User has delivered at least 5 doses and paired the app</t>
+  </si>
+  <si>
+    <t>System in use for 30 days</t>
+  </si>
+  <si>
+    <t>Patient data available</t>
+  </si>
+  <si>
+    <t>Critical alert triggered</t>
+  </si>
+  <si>
+    <t>Account exists</t>
+  </si>
+  <si>
+    <t>Account linked to email</t>
+  </si>
+  <si>
+    <t>Valid credentials existxists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Battery level is below 10%</t>
+  </si>
+  <si>
+    <t>Device is paired with the mobile app and powered on</t>
+  </si>
+  <si>
+    <t>1. Open the mobile app
+2. Navigate to device status section</t>
+  </si>
+  <si>
+    <t>1. Activate insulin delivery
+2. Observe system behavior</t>
+  </si>
+  <si>
+    <t>1. Open mobile app
+2. Check dosage and battery level</t>
+  </si>
+  <si>
+    <t>System delivers the configured insulin dose accurately</t>
+  </si>
+  <si>
+    <t>Last 5 doses and battery level are displayed</t>
+  </si>
+  <si>
+    <t>Current battery level of the device is displayed</t>
+  </si>
+  <si>
+    <t>System alerts user of low battery</t>
+  </si>
+  <si>
+    <t>1. Use device until battery &lt;10%
+2. Observe alert</t>
+  </si>
+  <si>
+    <t>1. Access dosage history
+2. Review records</t>
+  </si>
+  <si>
+    <t>30 days of dosage history is available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	1. Access storage
+2. Inspect encryption</t>
+  </si>
+  <si>
+    <t>Patient data is encrypted and stored locally</t>
+  </si>
+  <si>
+    <t>1. Trigger critical alert
+2. Observe device</t>
+  </si>
+  <si>
+    <t>Device notifies with vibration and LED</t>
+  </si>
+  <si>
+    <t>1. Enter username/password
+2. Click login</t>
+  </si>
+  <si>
+    <t>Login is successful</t>
+  </si>
+  <si>
+    <t>1. Enter username and wrong password
+2. Click login</t>
+  </si>
+  <si>
+    <t>Login fails and error message shown</t>
+  </si>
+  <si>
+    <t>1. Click "Forgot Password"
+2. Follow reset link</t>
+  </si>
+  <si>
+    <t>User can reset password successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,7 +238,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -440,20 +546,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="70.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="67" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="43.5" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -464,76 +570,216 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>